<commit_message>
time update and detail analysis 1.W
</commit_message>
<xml_diff>
--- a/LargeScaleAnalysis/01/WalkthroughDataComparison.xlsx
+++ b/LargeScaleAnalysis/01/WalkthroughDataComparison.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Walkthrough" sheetId="1" r:id="rId1"/>
     <sheet name="Game" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Results - Radii 7" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2492" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="932">
   <si>
     <t>###############1###############</t>
   </si>
@@ -2779,13 +2779,49 @@
   </si>
   <si>
     <t xml:space="preserve">01 1 004 Down  </t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>SF = 0.9    Radius = 7   Eta = 0.25
+Iterations = 100</t>
+  </si>
+  <si>
+    <t>SF = 0.5    Radius = 7   Eta = 0.25
+Iterations = 100</t>
+  </si>
+  <si>
+    <t>SF = 0.7    Radius = 7   Eta = 0.25
+Iterations = 100</t>
+  </si>
+  <si>
+    <t>GAME MODE (Radii = 7)</t>
+  </si>
+  <si>
+    <t>WALKTHROUGH MODE (Radii = 7)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>X = No Move of that type in Game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2793,8 +2829,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2813,8 +2865,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2822,19 +2880,179 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -2853,76 +3071,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -47282,22 +47430,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="P2:Q2 P3:P705 Q3:Q707">
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="T">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="T">
       <formula>NOT(ISERROR(SEARCH("T",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q707">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R704">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S704">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47310,8 +47458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A363" workbookViewId="0">
-      <selection activeCell="A378" sqref="A378"/>
+    <sheetView topLeftCell="A513" workbookViewId="0">
+      <selection activeCell="U526" sqref="U526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -80534,22 +80682,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="P2:P537">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q537">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R537">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S537">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -80560,12 +80708,904 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" customWidth="1"/>
+    <col min="18" max="18" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>929</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="19"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="19"/>
+    </row>
+    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>926</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="H3" s="8" t="s">
+        <v>927</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
+      <c r="N3" s="8" t="s">
+        <v>925</v>
+      </c>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="10"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="13"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="22">
+        <v>4</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="22">
+        <v>3</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="7">
+        <v>2</v>
+      </c>
+      <c r="N7" s="7">
+        <v>1</v>
+      </c>
+      <c r="O7" s="22">
+        <v>3</v>
+      </c>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="7">
+        <v>3</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22">
+        <v>5</v>
+      </c>
+      <c r="H8" s="7">
+        <v>2</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="7">
+        <v>4</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="L8" s="22">
+        <v>6</v>
+      </c>
+      <c r="N8" s="7">
+        <v>2</v>
+      </c>
+      <c r="O8" s="21"/>
+      <c r="P8" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>3</v>
+      </c>
+      <c r="C9" s="22">
+        <v>7</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="H9" s="7">
+        <v>3</v>
+      </c>
+      <c r="I9" s="22">
+        <v>8</v>
+      </c>
+      <c r="J9" s="21"/>
+      <c r="K9" s="7">
+        <v>1</v>
+      </c>
+      <c r="L9" s="21"/>
+      <c r="N9" s="7">
+        <v>3</v>
+      </c>
+      <c r="O9" s="22">
+        <v>5</v>
+      </c>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="22">
+        <v>6</v>
+      </c>
+      <c r="R9" s="21"/>
+    </row>
+    <row r="10" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>4</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="H10" s="7">
+        <v>4</v>
+      </c>
+      <c r="I10" s="21"/>
+      <c r="J10" s="7">
+        <v>4</v>
+      </c>
+      <c r="K10" s="7">
+        <v>1</v>
+      </c>
+      <c r="L10" s="21"/>
+      <c r="N10" s="7">
+        <v>4</v>
+      </c>
+      <c r="O10" s="21"/>
+      <c r="P10" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>2</v>
+      </c>
+      <c r="R10" s="21"/>
+      <c r="T10" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="7">
+        <v>2</v>
+      </c>
+      <c r="H11" s="7">
+        <v>5</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <v>4</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="7">
+        <v>2</v>
+      </c>
+      <c r="N11" s="7">
+        <v>5</v>
+      </c>
+      <c r="O11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
+        <v>6</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="22">
+        <v>6</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="H12" s="7">
+        <v>6</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
+      <c r="J12" s="22">
+        <v>7</v>
+      </c>
+      <c r="K12" s="7">
+        <v>1</v>
+      </c>
+      <c r="L12" s="21"/>
+      <c r="N12" s="7">
+        <v>6</v>
+      </c>
+      <c r="O12" s="7">
+        <v>0</v>
+      </c>
+      <c r="P12" s="22">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>2</v>
+      </c>
+      <c r="R12" s="21"/>
+    </row>
+    <row r="13" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2</v>
+      </c>
+      <c r="H13" s="7">
+        <v>7</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22">
+        <v>5</v>
+      </c>
+      <c r="L13" s="7">
+        <v>2</v>
+      </c>
+      <c r="N13" s="7">
+        <v>7</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="22">
+        <v>8</v>
+      </c>
+      <c r="R13" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
+        <v>8</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="7">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
+      <c r="H14" s="7">
+        <v>8</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="7">
+        <v>4</v>
+      </c>
+      <c r="K14" s="7">
+        <v>1</v>
+      </c>
+      <c r="L14" s="7">
+        <v>2</v>
+      </c>
+      <c r="N14" s="7">
+        <v>8</v>
+      </c>
+      <c r="O14" s="21"/>
+      <c r="P14" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>2</v>
+      </c>
+      <c r="R14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>3</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7">
+        <v>2</v>
+      </c>
+      <c r="H15" s="7">
+        <v>9</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>4</v>
+      </c>
+      <c r="K15" s="7">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7">
+        <v>2</v>
+      </c>
+      <c r="N15" s="7">
+        <v>9</v>
+      </c>
+      <c r="O15" s="7">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>2</v>
+      </c>
+      <c r="R15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>928</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>926</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="H18" s="8" t="s">
+        <v>927</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="10"/>
+      <c r="N18" s="8" t="s">
+        <v>925</v>
+      </c>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="10"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="13"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="13"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="16"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="7">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="3"/>
+      <c r="N22" s="7">
+        <v>1</v>
+      </c>
+      <c r="O22" s="3"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="3"/>
+    </row>
+    <row r="23" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="3"/>
+      <c r="H23" s="7">
+        <v>2</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="3"/>
+      <c r="N23" s="7">
+        <v>2</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="6"/>
+      <c r="H24" s="7">
+        <v>3</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="6"/>
+      <c r="N24" s="7">
+        <v>3</v>
+      </c>
+      <c r="O24" s="3"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="6"/>
+    </row>
+    <row r="25" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="6"/>
+      <c r="H25" s="7">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="6"/>
+      <c r="N25" s="7">
+        <v>4</v>
+      </c>
+      <c r="O25" s="6"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="6"/>
+    </row>
+    <row r="26" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="3"/>
+      <c r="H26" s="7">
+        <v>5</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="3"/>
+      <c r="N26" s="7">
+        <v>5</v>
+      </c>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="6"/>
+      <c r="H27" s="7">
+        <v>6</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="6"/>
+      <c r="N27" s="7">
+        <v>6</v>
+      </c>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="6"/>
+    </row>
+    <row r="28" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
+        <v>7</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="H28" s="7">
+        <v>7</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="N28" s="7">
+        <v>7</v>
+      </c>
+      <c r="O28" s="3"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+    </row>
+    <row r="29" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
+        <v>8</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="7">
+        <v>8</v>
+      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="N29" s="7">
+        <v>8</v>
+      </c>
+      <c r="O29" s="6"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+    </row>
+    <row r="30" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
+        <v>9</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="H30" s="7">
+        <v>9</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="N30" s="7">
+        <v>9</v>
+      </c>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B18:F20"/>
+    <mergeCell ref="H18:L20"/>
+    <mergeCell ref="N18:R20"/>
+    <mergeCell ref="A1:S2"/>
+    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B3:F5"/>
+    <mergeCell ref="H3:L5"/>
+    <mergeCell ref="N3:R5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>